<commit_message>
New data: length of stay
</commit_message>
<xml_diff>
--- a/data/Dex_metan.xlsx
+++ b/data/Dex_metan.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BD5A50-879C-8A41-A0AD-1319A90ECB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC23DBF-5863-644C-AB4D-9D29C26C3EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="23480" windowHeight="16320" xr2:uid="{8A3D6ABD-EAAB-5E44-A89E-74340099A36C}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="21320" windowHeight="16320" xr2:uid="{8A3D6ABD-EAAB-5E44-A89E-74340099A36C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="48">
   <si>
     <t>Shi et al</t>
   </si>
@@ -141,6 +141,45 @@
   </si>
   <si>
     <t>FEV1 POD 2</t>
+  </si>
+  <si>
+    <t>LOS</t>
+  </si>
+  <si>
+    <t>4.10 ± 1.48</t>
+  </si>
+  <si>
+    <t>4.60 ± 1.88</t>
+  </si>
+  <si>
+    <t>7.10 ± 3.90</t>
+  </si>
+  <si>
+    <t>7.76 ± 3.12</t>
+  </si>
+  <si>
+    <t>5.60 ± 2.50</t>
+  </si>
+  <si>
+    <t>5.90 ± 2.50</t>
+  </si>
+  <si>
+    <t>6.33 ± 4.61</t>
+  </si>
+  <si>
+    <t>9.66 ± 5.38</t>
+  </si>
+  <si>
+    <t>7.16 ± 3.93</t>
+  </si>
+  <si>
+    <t>8.03 ± 3.93</t>
+  </si>
+  <si>
+    <t>6.10 ± 4.58</t>
+  </si>
+  <si>
+    <t>7.13 ± 3.81</t>
   </si>
 </sst>
 </file>
@@ -172,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,17 +228,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE8882F-013A-C84A-9D48-47B509BAD197}">
-  <dimension ref="B1:T64"/>
+  <dimension ref="B1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65:K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,6 +1782,221 @@
         <v>34</v>
       </c>
     </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D67">
+        <v>1.48</v>
+      </c>
+      <c r="E67">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F67">
+        <v>1.88</v>
+      </c>
+      <c r="G67">
+        <v>20</v>
+      </c>
+      <c r="H67">
+        <v>20</v>
+      </c>
+      <c r="I67" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" t="s">
+        <v>36</v>
+      </c>
+      <c r="K67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <v>7.1</v>
+      </c>
+      <c r="D68">
+        <v>3.9</v>
+      </c>
+      <c r="E68">
+        <v>7.76</v>
+      </c>
+      <c r="F68">
+        <v>3.12</v>
+      </c>
+      <c r="G68">
+        <v>28</v>
+      </c>
+      <c r="H68">
+        <v>28</v>
+      </c>
+      <c r="I68" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" t="s">
+        <v>38</v>
+      </c>
+      <c r="K68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>5.6</v>
+      </c>
+      <c r="D69">
+        <v>2.5</v>
+      </c>
+      <c r="E69">
+        <v>5.9</v>
+      </c>
+      <c r="F69">
+        <v>2.5</v>
+      </c>
+      <c r="G69">
+        <v>30</v>
+      </c>
+      <c r="H69">
+        <v>30</v>
+      </c>
+      <c r="I69" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" t="s">
+        <v>40</v>
+      </c>
+      <c r="K69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>6.33</v>
+      </c>
+      <c r="D70">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E70">
+        <v>9.66</v>
+      </c>
+      <c r="F70">
+        <v>5.38</v>
+      </c>
+      <c r="G70">
+        <v>40</v>
+      </c>
+      <c r="H70">
+        <v>40</v>
+      </c>
+      <c r="I70" t="s">
+        <v>35</v>
+      </c>
+      <c r="J70" t="s">
+        <v>42</v>
+      </c>
+      <c r="K70" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71">
+        <v>7.16</v>
+      </c>
+      <c r="D71">
+        <v>3.93</v>
+      </c>
+      <c r="E71">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F71">
+        <v>3.93</v>
+      </c>
+      <c r="G71">
+        <v>25</v>
+      </c>
+      <c r="H71">
+        <v>25</v>
+      </c>
+      <c r="I71" t="s">
+        <v>35</v>
+      </c>
+      <c r="J71" t="s">
+        <v>44</v>
+      </c>
+      <c r="K71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>6.1</v>
+      </c>
+      <c r="D72">
+        <v>4.58</v>
+      </c>
+      <c r="E72">
+        <v>7.13</v>
+      </c>
+      <c r="F72">
+        <v>3.81</v>
+      </c>
+      <c r="G72">
+        <v>50</v>
+      </c>
+      <c r="H72">
+        <v>50</v>
+      </c>
+      <c r="I72" t="s">
+        <v>35</v>
+      </c>
+      <c r="J72" t="s">
+        <v>46</v>
+      </c>
+      <c r="K72" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Added length of stay (Sec'y)
</commit_message>
<xml_diff>
--- a/data/Dex_metan.xlsx
+++ b/data/Dex_metan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC23DBF-5863-644C-AB4D-9D29C26C3EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C4ED25-279E-E14A-9E08-4B4143246BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="21320" windowHeight="16320" xr2:uid="{8A3D6ABD-EAAB-5E44-A89E-74340099A36C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="104">
   <si>
     <t>Shi et al</t>
   </si>
@@ -180,6 +180,174 @@
   </si>
   <si>
     <t>7.13 ± 3.81</t>
+  </si>
+  <si>
+    <t>Quingming et al (1)</t>
+  </si>
+  <si>
+    <t>Quingming et al (2)</t>
+  </si>
+  <si>
+    <t>1.7% (1/60)</t>
+  </si>
+  <si>
+    <t>5.0% (3/60)</t>
+  </si>
+  <si>
+    <t>0.0% (0/58)</t>
+  </si>
+  <si>
+    <t>3.4% (2/58)</t>
+  </si>
+  <si>
+    <t>5.0% (1/20)</t>
+  </si>
+  <si>
+    <t>10.0% (2/20)</t>
+  </si>
+  <si>
+    <t>14.3% (4/28)</t>
+  </si>
+  <si>
+    <t>7.5% (3/40)</t>
+  </si>
+  <si>
+    <t>5.0% (2/40)</t>
+  </si>
+  <si>
+    <t>0.0% (0/25)</t>
+  </si>
+  <si>
+    <t>0.0% (0/28)</t>
+  </si>
+  <si>
+    <t>16.0% (4/25)</t>
+  </si>
+  <si>
+    <t>4.0% (2/50)</t>
+  </si>
+  <si>
+    <t>6.0% (3/50)</t>
+  </si>
+  <si>
+    <t>1.7% (1/59)</t>
+  </si>
+  <si>
+    <t>5.7% (3/53)</t>
+  </si>
+  <si>
+    <t>0.0% (0/20)</t>
+  </si>
+  <si>
+    <t>6.7% (4/60)</t>
+  </si>
+  <si>
+    <t>1.7% (1/58)</t>
+  </si>
+  <si>
+    <t>6.9% (4/58)</t>
+  </si>
+  <si>
+    <t>0.0% (0/30)</t>
+  </si>
+  <si>
+    <t>3.3% (1/30)</t>
+  </si>
+  <si>
+    <t>2.0% (1/50)</t>
+  </si>
+  <si>
+    <t>20.0% (12/60)</t>
+  </si>
+  <si>
+    <t>7.5% (4/53)</t>
+  </si>
+  <si>
+    <t>3.3% (2/60)</t>
+  </si>
+  <si>
+    <t>3.6% (1/28)</t>
+  </si>
+  <si>
+    <t>4.0% (1/25)</t>
+  </si>
+  <si>
+    <t>19.2 ± 2.8</t>
+  </si>
+  <si>
+    <t>19.9 ± 3.8</t>
+  </si>
+  <si>
+    <t>18.2 ± 3.2</t>
+  </si>
+  <si>
+    <t>23.0 ± 4.1</t>
+  </si>
+  <si>
+    <t>18.6 ± 2.1</t>
+  </si>
+  <si>
+    <t>21.3 ± 3.2</t>
+  </si>
+  <si>
+    <t>22.6 ± 3.1</t>
+  </si>
+  <si>
+    <t>23.4 ± 3.3</t>
+  </si>
+  <si>
+    <t>19.2 ± 2.2</t>
+  </si>
+  <si>
+    <t>20.0 ± 2.6</t>
+  </si>
+  <si>
+    <t>20.8 ± 4.0</t>
+  </si>
+  <si>
+    <t>21.9 ± 3.6</t>
+  </si>
+  <si>
+    <t>17.8 ± 3.5</t>
+  </si>
+  <si>
+    <t>23.5 ± 4.8</t>
+  </si>
+  <si>
+    <t>24.6 ± 3.1</t>
+  </si>
+  <si>
+    <t>25.6 ± 3.2</t>
+  </si>
+  <si>
+    <t>21.3 ± 2.3</t>
+  </si>
+  <si>
+    <t>22.1 ± 2.6</t>
+  </si>
+  <si>
+    <t>23.2 ± 5.3</t>
+  </si>
+  <si>
+    <t>18.7 ± 4.6</t>
+  </si>
+  <si>
+    <t>22.5 ± 3.5</t>
+  </si>
+  <si>
+    <t>17.7 ± 3.4</t>
+  </si>
+  <si>
+    <t>29.4 ± 2.8</t>
+  </si>
+  <si>
+    <t>28.1 ± 5.0</t>
+  </si>
+  <si>
+    <t>32.0 ± 3.7</t>
+  </si>
+  <si>
+    <t>29.1 ± 6.7</t>
   </si>
 </sst>
 </file>
@@ -241,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,6 +417,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,56 +736,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE8882F-013A-C84A-9D48-47B509BAD197}">
-  <dimension ref="B1:T73"/>
+  <dimension ref="B1:AB79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65:K73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" activeCellId="2" sqref="D3 D4 D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="15.5" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="10" width="16" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="20" max="20" width="15.5" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="3"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="2:28" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>22</v>
       </c>
@@ -623,36 +805,24 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
       <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" t="s">
         <v>29</v>
       </c>
       <c r="Q2" t="s">
@@ -667,8 +837,20 @@
       <c r="T2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="W2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -692,48 +874,72 @@
         <f>D3-F3</f>
         <v>57</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3">
         <v>3</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>4</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>57</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>56</v>
       </c>
-      <c r="M3">
+      <c r="O3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3">
         <v>4</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>12</v>
-      </c>
-      <c r="O3">
-        <f>C3-M3</f>
-        <v>56</v>
-      </c>
-      <c r="P3">
-        <f>D3-N3</f>
-        <v>48</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
       </c>
       <c r="S3">
         <f>C3-Q3</f>
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="T3">
         <f>D3-R3</f>
+        <v>48</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <f>C3-W3</f>
+        <v>59</v>
+      </c>
+      <c r="Z3">
+        <f>D3-X3</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -754,37 +960,55 @@
         <v>58</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H11" si="1">D4-F4</f>
+        <f t="shared" ref="H4:H10" si="1">D4-F4</f>
         <v>56</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>4</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>57</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>54</v>
       </c>
-      <c r="M4">
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="R4">
         <v>4</v>
       </c>
-      <c r="O4">
-        <f>C4-M4</f>
+      <c r="S4">
+        <f>C4-Q4</f>
         <v>57</v>
       </c>
-      <c r="P4">
-        <f>D4-N4</f>
+      <c r="T4">
+        <f>D4-R4</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -808,20 +1032,32 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>18</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -845,45 +1081,57 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="Q6">
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6">
         <v>0</v>
       </c>
-      <c r="R6">
+      <c r="X6">
         <v>1</v>
       </c>
-      <c r="S6">
-        <f>C6-Q6</f>
+      <c r="Y6">
+        <f>C6-W6</f>
         <v>28</v>
       </c>
-      <c r="T6">
-        <f>D6-R6</f>
+      <c r="Z6">
+        <f>D6-X6</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
         <v>30</v>
       </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>30</v>
-      </c>
-      <c r="L7">
+      <c r="N7">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -907,20 +1155,32 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>38</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -944,22 +1204,34 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="Q9">
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9">
         <v>0</v>
       </c>
-      <c r="R9">
+      <c r="X9">
         <v>1</v>
       </c>
-      <c r="S9">
-        <f>C9-Q9</f>
+      <c r="Y9">
+        <f>C9-W9</f>
         <v>25</v>
       </c>
-      <c r="T9">
-        <f>D9-R9</f>
+      <c r="Z9">
+        <f>D9-X9</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -983,20 +1255,32 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>2</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>49</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1017,96 +1301,238 @@
         <v>58</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f>D11-F11</f>
         <v>50</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>3</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>58</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>50</v>
       </c>
-      <c r="M11">
+      <c r="O11" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q11">
         <v>1</v>
       </c>
-      <c r="N11">
+      <c r="R11">
         <v>4</v>
       </c>
-      <c r="O11">
-        <f>C11-M11</f>
+      <c r="S11">
+        <f>C11-Q11</f>
         <v>58</v>
       </c>
-      <c r="P11">
-        <f>D11-N11</f>
+      <c r="T11">
+        <f>D11-R11</f>
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U11" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>19</v>
+      </c>
+      <c r="N12">
+        <v>19</v>
+      </c>
+      <c r="O12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>20</v>
+      </c>
+      <c r="T12">
+        <v>19</v>
+      </c>
+      <c r="U12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>20</v>
+      </c>
+      <c r="T13">
+        <v>19</v>
+      </c>
+      <c r="U13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H16" t="s">
         <v>10</v>
       </c>
+      <c r="K16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>19.2</v>
+      </c>
+      <c r="D17">
+        <v>2.8</v>
+      </c>
+      <c r="E17">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F17">
+        <v>3.8</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
       <c r="I17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="J17" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>19.2</v>
-      </c>
-      <c r="D18">
-        <v>2.8</v>
-      </c>
-      <c r="E18">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F18">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="H18">
-        <v>60</v>
-      </c>
-      <c r="I18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1116,11 +1542,11 @@
       <c r="H19">
         <v>58</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1130,11 +1556,11 @@
       <c r="H20">
         <v>20</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1144,11 +1570,11 @@
       <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -1158,11 +1584,11 @@
       <c r="H22">
         <v>30</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -1172,11 +1598,11 @@
       <c r="H23">
         <v>40</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1199,10 +1625,16 @@
         <v>25</v>
       </c>
       <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -1212,11 +1644,11 @@
       <c r="H25">
         <v>50</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -1226,691 +1658,780 @@
       <c r="H26">
         <v>53</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" t="s">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="6">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="E28" s="6">
+        <v>21.3</v>
+      </c>
+      <c r="F28" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>62</v>
+      </c>
+      <c r="H28" s="6">
+        <v>62</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="1">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="E29" s="1">
-        <v>21.3</v>
-      </c>
-      <c r="F29" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="G29" s="1">
-        <v>62</v>
-      </c>
-      <c r="H29" s="1">
-        <v>62</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="6">
+        <v>22.6</v>
+      </c>
+      <c r="D30" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>23.4</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="G30" s="7">
+        <v>20</v>
+      </c>
+      <c r="H30" s="7">
+        <v>20</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K30" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E31" s="1">
+        <v>20</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20</v>
+      </c>
+      <c r="H31" s="1">
+        <v>20</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>20.8</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>4</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <v>21.9</v>
       </c>
-      <c r="F30">
+      <c r="F32">
         <v>3.6</v>
       </c>
-      <c r="G30">
+      <c r="G32">
         <v>60</v>
       </c>
-      <c r="H30">
+      <c r="H32">
         <v>60</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I32" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <v>58</v>
       </c>
-      <c r="H31">
+      <c r="H33">
         <v>58</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>2</v>
       </c>
-      <c r="G32">
-        <v>20</v>
-      </c>
-      <c r="H32">
-        <v>20</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="G34">
+        <v>20</v>
+      </c>
+      <c r="H34">
+        <v>20</v>
+      </c>
+      <c r="K34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>3</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>17.8</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>3.5</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <v>23.5</v>
       </c>
-      <c r="F33">
+      <c r="F35">
         <v>4.8</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <v>28</v>
       </c>
-      <c r="H33">
+      <c r="H35">
         <v>28</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>4</v>
       </c>
-      <c r="G34">
+      <c r="G36">
         <v>30</v>
       </c>
-      <c r="H34">
+      <c r="H36">
         <v>30</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="G35">
+      <c r="G37">
         <v>40</v>
       </c>
-      <c r="H35">
+      <c r="H37">
         <v>40</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="G36">
+      <c r="G38">
         <v>25</v>
       </c>
-      <c r="H36">
+      <c r="H38">
         <v>25</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37">
-        <v>50</v>
-      </c>
-      <c r="H37">
-        <v>50</v>
-      </c>
-      <c r="I37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38">
-        <v>59</v>
-      </c>
-      <c r="H38">
-        <v>53</v>
-      </c>
-      <c r="I38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="I39" t="s">
+      <c r="G39">
+        <v>50</v>
+      </c>
+      <c r="H39">
+        <v>50</v>
+      </c>
+      <c r="K39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>59</v>
+      </c>
+      <c r="H40">
+        <v>53</v>
+      </c>
+      <c r="K40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>11</v>
       </c>
-      <c r="I40" t="s">
+      <c r="K42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1">
+      <c r="G43" s="1">
         <v>62</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H43" s="1">
         <v>62</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="K43" t="s">
         <v>19</v>
       </c>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>24.6</v>
+      </c>
+      <c r="D44">
+        <v>3.1</v>
+      </c>
+      <c r="E44">
+        <v>25.6</v>
+      </c>
+      <c r="F44">
+        <v>3.2</v>
+      </c>
+      <c r="G44" s="7">
+        <v>20</v>
+      </c>
+      <c r="H44" s="7">
+        <v>20</v>
+      </c>
+      <c r="I44" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44" t="s">
+        <v>93</v>
+      </c>
+      <c r="K44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E45" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="G45" s="1">
+        <v>20</v>
+      </c>
+      <c r="H45" s="1">
+        <v>20</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>0</v>
       </c>
-      <c r="G42">
+      <c r="G46">
         <v>60</v>
       </c>
-      <c r="H42">
+      <c r="H46">
         <v>60</v>
       </c>
-      <c r="I42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+      <c r="K46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="G43">
+      <c r="G47">
         <v>58</v>
       </c>
-      <c r="H43">
+      <c r="H47">
         <v>58</v>
       </c>
-      <c r="I43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="K47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>2</v>
       </c>
-      <c r="G44">
-        <v>20</v>
-      </c>
-      <c r="H44">
-        <v>20</v>
-      </c>
-      <c r="I44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+      <c r="G48">
+        <v>20</v>
+      </c>
+      <c r="H48">
+        <v>20</v>
+      </c>
+      <c r="K48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>3</v>
       </c>
-      <c r="C45">
+      <c r="C49">
         <v>23.2</v>
       </c>
-      <c r="D45">
+      <c r="D49">
         <v>5.3</v>
       </c>
-      <c r="E45">
+      <c r="E49">
         <v>18.7</v>
       </c>
-      <c r="F45">
+      <c r="F49">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G45">
+      <c r="G49">
         <v>28</v>
       </c>
-      <c r="H45">
+      <c r="H49">
         <v>28</v>
       </c>
-      <c r="I45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+      <c r="I49" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" t="s">
+        <v>97</v>
+      </c>
+      <c r="K49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>4</v>
       </c>
-      <c r="G46">
+      <c r="G50">
         <v>30</v>
       </c>
-      <c r="H46">
+      <c r="H50">
         <v>30</v>
       </c>
-      <c r="I46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="K50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>5</v>
       </c>
-      <c r="G47">
+      <c r="G51">
         <v>40</v>
       </c>
-      <c r="H47">
+      <c r="H51">
         <v>40</v>
       </c>
-      <c r="I47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+      <c r="K51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>6</v>
       </c>
-      <c r="C48">
+      <c r="C52">
         <v>22.5</v>
       </c>
-      <c r="D48">
+      <c r="D52">
         <v>3.5</v>
       </c>
-      <c r="E48">
+      <c r="E52">
         <v>17.7</v>
       </c>
-      <c r="F48">
+      <c r="F52">
         <v>3.4</v>
       </c>
-      <c r="G48">
+      <c r="G52">
         <v>25</v>
       </c>
-      <c r="H48">
+      <c r="H52">
         <v>25</v>
       </c>
-      <c r="I48" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+      <c r="I52" t="s">
+        <v>98</v>
+      </c>
+      <c r="J52" t="s">
+        <v>99</v>
+      </c>
+      <c r="K52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>7</v>
       </c>
-      <c r="G49">
+      <c r="G53">
         <v>50</v>
       </c>
-      <c r="H49">
+      <c r="H53">
         <v>50</v>
       </c>
-      <c r="I49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+      <c r="K53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>8</v>
       </c>
-      <c r="G50">
+      <c r="G54">
         <v>59</v>
       </c>
-      <c r="H50">
+      <c r="H54">
         <v>53</v>
       </c>
-      <c r="I50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+      <c r="K54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="I51" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+      <c r="K55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>11</v>
       </c>
-      <c r="I52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+      <c r="K56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1">
         <v>62</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H57" s="1">
         <v>62</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58">
+        <v>29.4</v>
+      </c>
+      <c r="D58">
+        <v>2.8</v>
+      </c>
+      <c r="E58">
+        <v>28.1</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+      <c r="G58" s="7">
+        <v>20</v>
+      </c>
+      <c r="H58" s="7">
+        <v>20</v>
+      </c>
+      <c r="I58" t="s">
+        <v>100</v>
+      </c>
+      <c r="J58" t="s">
+        <v>101</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="1">
+        <v>32</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="E59" s="1">
+        <v>29.1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="G59" s="1">
+        <v>20</v>
+      </c>
+      <c r="H59" s="1">
+        <v>20</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="6"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
         <v>5</v>
       </c>
-      <c r="C59">
+      <c r="C65">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D59">
+      <c r="D65">
         <v>0.4</v>
       </c>
-      <c r="E59">
+      <c r="E65">
         <v>1.8</v>
       </c>
-      <c r="F59">
+      <c r="F65">
         <v>0.5</v>
       </c>
-      <c r="G59">
+      <c r="G65">
         <v>40</v>
       </c>
-      <c r="H59">
+      <c r="H65">
         <v>40</v>
       </c>
-      <c r="I59" t="s">
+      <c r="K65" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>7</v>
       </c>
-      <c r="C61">
+      <c r="C67">
         <v>2.1</v>
       </c>
-      <c r="D61">
+      <c r="D67">
         <v>0.4</v>
       </c>
-      <c r="E61">
+      <c r="E67">
         <v>1.9</v>
       </c>
-      <c r="F61">
+      <c r="F67">
         <v>0.5</v>
       </c>
-      <c r="G61">
+      <c r="G67">
         <v>50</v>
       </c>
-      <c r="H61">
+      <c r="H67">
         <v>50</v>
       </c>
-      <c r="I61" t="s">
+      <c r="K67" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
         <v>7</v>
       </c>
-      <c r="C63">
+      <c r="C69">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D63">
+      <c r="D69">
         <v>0.5</v>
       </c>
-      <c r="E63">
+      <c r="E69">
         <v>2</v>
       </c>
-      <c r="F63">
+      <c r="F69">
         <v>0.4</v>
       </c>
-      <c r="G63">
+      <c r="G69">
         <v>50</v>
       </c>
-      <c r="H63">
+      <c r="H69">
         <v>50</v>
       </c>
-      <c r="I63" t="s">
+      <c r="K69" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D64">
-        <v>0.5</v>
-      </c>
-      <c r="E64">
-        <v>2</v>
-      </c>
-      <c r="F64">
-        <v>0.3</v>
-      </c>
-      <c r="G64">
-        <v>40</v>
-      </c>
-      <c r="H64">
-        <v>40</v>
-      </c>
-      <c r="I64" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D67">
-        <v>1.48</v>
-      </c>
-      <c r="E67">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F67">
-        <v>1.88</v>
-      </c>
-      <c r="G67">
-        <v>20</v>
-      </c>
-      <c r="H67">
-        <v>20</v>
-      </c>
-      <c r="I67" t="s">
-        <v>35</v>
-      </c>
-      <c r="J67" t="s">
-        <v>36</v>
-      </c>
-      <c r="K67" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68">
-        <v>7.1</v>
-      </c>
-      <c r="D68">
-        <v>3.9</v>
-      </c>
-      <c r="E68">
-        <v>7.76</v>
-      </c>
-      <c r="F68">
-        <v>3.12</v>
-      </c>
-      <c r="G68">
-        <v>28</v>
-      </c>
-      <c r="H68">
-        <v>28</v>
-      </c>
-      <c r="I68" t="s">
-        <v>35</v>
-      </c>
-      <c r="J68" t="s">
-        <v>38</v>
-      </c>
-      <c r="K68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69">
-        <v>5.6</v>
-      </c>
-      <c r="D69">
-        <v>2.5</v>
-      </c>
-      <c r="E69">
-        <v>5.9</v>
-      </c>
-      <c r="F69">
-        <v>2.5</v>
-      </c>
-      <c r="G69">
-        <v>30</v>
-      </c>
-      <c r="H69">
-        <v>30</v>
-      </c>
-      <c r="I69" t="s">
-        <v>35</v>
-      </c>
-      <c r="J69" t="s">
-        <v>40</v>
-      </c>
-      <c r="K69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>5</v>
       </c>
       <c r="C70">
-        <v>6.33</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D70">
-        <v>4.6100000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="E70">
-        <v>9.66</v>
+        <v>2</v>
       </c>
       <c r="F70">
-        <v>5.38</v>
+        <v>0.3</v>
       </c>
       <c r="G70">
         <v>40</v>
@@ -1918,82 +2439,224 @@
       <c r="H70">
         <v>40</v>
       </c>
-      <c r="I70" t="s">
+      <c r="K70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D73">
+        <v>1.48</v>
+      </c>
+      <c r="E73">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F73">
+        <v>1.88</v>
+      </c>
+      <c r="G73">
+        <v>20</v>
+      </c>
+      <c r="H73">
+        <v>20</v>
+      </c>
+      <c r="K73" t="s">
         <v>35</v>
       </c>
-      <c r="J70" t="s">
+      <c r="L73" t="s">
+        <v>36</v>
+      </c>
+      <c r="M73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74">
+        <v>7.1</v>
+      </c>
+      <c r="D74">
+        <v>3.9</v>
+      </c>
+      <c r="E74">
+        <v>7.76</v>
+      </c>
+      <c r="F74">
+        <v>3.12</v>
+      </c>
+      <c r="G74">
+        <v>28</v>
+      </c>
+      <c r="H74">
+        <v>28</v>
+      </c>
+      <c r="K74" t="s">
+        <v>35</v>
+      </c>
+      <c r="L74" t="s">
+        <v>38</v>
+      </c>
+      <c r="M74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>5.6</v>
+      </c>
+      <c r="D75">
+        <v>2.5</v>
+      </c>
+      <c r="E75">
+        <v>5.9</v>
+      </c>
+      <c r="F75">
+        <v>2.5</v>
+      </c>
+      <c r="G75">
+        <v>30</v>
+      </c>
+      <c r="H75">
+        <v>30</v>
+      </c>
+      <c r="K75" t="s">
+        <v>35</v>
+      </c>
+      <c r="L75" t="s">
+        <v>40</v>
+      </c>
+      <c r="M75" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>6.33</v>
+      </c>
+      <c r="D76">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E76">
+        <v>9.66</v>
+      </c>
+      <c r="F76">
+        <v>5.38</v>
+      </c>
+      <c r="G76">
+        <v>40</v>
+      </c>
+      <c r="H76">
+        <v>40</v>
+      </c>
+      <c r="K76" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" t="s">
         <v>42</v>
       </c>
-      <c r="K70" t="s">
+      <c r="M76" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>6</v>
       </c>
-      <c r="C71">
+      <c r="C77">
         <v>7.16</v>
       </c>
-      <c r="D71">
+      <c r="D77">
         <v>3.93</v>
       </c>
-      <c r="E71">
+      <c r="E77">
         <v>8.0299999999999994</v>
       </c>
-      <c r="F71">
+      <c r="F77">
         <v>3.93</v>
       </c>
-      <c r="G71">
+      <c r="G77">
         <v>25</v>
       </c>
-      <c r="H71">
+      <c r="H77">
         <v>25</v>
       </c>
-      <c r="I71" t="s">
+      <c r="K77" t="s">
         <v>35</v>
       </c>
-      <c r="J71" t="s">
+      <c r="L77" t="s">
         <v>44</v>
       </c>
-      <c r="K71" t="s">
+      <c r="M77" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
         <v>7</v>
       </c>
-      <c r="C72">
+      <c r="C78">
         <v>6.1</v>
       </c>
-      <c r="D72">
+      <c r="D78">
         <v>4.58</v>
       </c>
-      <c r="E72">
+      <c r="E78">
         <v>7.13</v>
       </c>
-      <c r="F72">
+      <c r="F78">
         <v>3.81</v>
       </c>
-      <c r="G72">
+      <c r="G78">
         <v>50</v>
       </c>
-      <c r="H72">
+      <c r="H78">
         <v>50</v>
       </c>
-      <c r="I72" t="s">
+      <c r="K78" t="s">
         <v>35</v>
       </c>
-      <c r="J72" t="s">
+      <c r="L78" t="s">
         <v>46</v>
       </c>
-      <c r="K72" t="s">
+      <c r="M78" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2001,9 +2664,9 @@
   <mergeCells count="5">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="K1:N1"/>
     <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="W1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>